<commit_message>
Added 3 new skills in the Hunter doc. Only 1 remaning
</commit_message>
<xml_diff>
--- a/GameDesign/Class/Hunter/Documentation/HunterSkills.xlsx
+++ b/GameDesign/Class/Hunter/Documentation/HunterSkills.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="1" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="1-DistortionArea" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,9 @@
     <sheet name="4-PiercingArrow" sheetId="4" r:id="rId4"/>
     <sheet name="5-IgnitionArrow" sheetId="5" r:id="rId5"/>
     <sheet name="6-CursedArrow" sheetId="6" r:id="rId6"/>
-    <sheet name="Feuil1 (7)" sheetId="7" r:id="rId7"/>
-    <sheet name="Feuil1 (8)" sheetId="8" r:id="rId8"/>
-    <sheet name="Feuil1 (9)" sheetId="9" r:id="rId9"/>
+    <sheet name="7-PoisonArrow" sheetId="7" r:id="rId7"/>
+    <sheet name="8-Survival" sheetId="8" r:id="rId8"/>
+    <sheet name="9-CanisLupus" sheetId="9" r:id="rId9"/>
     <sheet name="Feuil1 (10)" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="171027"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="120">
   <si>
     <t>[[AP: 0 ]]</t>
   </si>
@@ -291,13 +291,115 @@
   </si>
   <si>
     <t>Self: If under ''Blood Mark'' effect, Unbuff ''Blood Mark'' effect.</t>
+  </si>
+  <si>
+    <t>Poison Arrow</t>
+  </si>
+  <si>
+    <t>If I have to sacrifice myself to eliminate you, so be it</t>
+  </si>
+  <si>
+    <t>[[Max effect accumulation: 3 ]]</t>
+  </si>
+  <si>
+    <t>[[Number of casts per turn: 2 ]]</t>
+  </si>
+  <si>
+    <t>[[Number of cast per turn per target: 1 ]]</t>
+  </si>
+  <si>
+    <t>[[Range: 1-5 ]]</t>
+  </si>
+  <si>
+    <t>If not under ''Blood Mark'' effect: [[Damage:  25 dark ]] (2 turns)</t>
+  </si>
+  <si>
+    <t>If under ''Blood Mark'' effect: [[Damage:  25 dark ]] (3 turns)</t>
+  </si>
+  <si>
+    <t>Effect name: ''Poison''.</t>
+  </si>
+  <si>
+    <t>Hidden in the darkness, I'll watch your life</t>
+  </si>
+  <si>
+    <t>leave your body slowly, but surely.</t>
+  </si>
+  <si>
+    <t>The hunter has become the prey, irony of fate…</t>
+  </si>
+  <si>
+    <t>Survival</t>
+  </si>
+  <si>
+    <t>[[AP: 6 ]]</t>
+  </si>
+  <si>
+    <t>[[Range: 0 ]]</t>
+  </si>
+  <si>
+    <t>[[Number of turns between two casts: 5 ]]</t>
+  </si>
+  <si>
+    <t>[[Boost MP by current iteself]] (1 turn)</t>
+  </si>
+  <si>
+    <t>[[Boost HP by 15% of max HP]] (3 turns)</t>
+  </si>
+  <si>
+    <t>Effect name: ''Survival''.</t>
+  </si>
+  <si>
+    <t>Usable only if has 25% or less HP.</t>
+  </si>
+  <si>
+    <t>Canis Lupus</t>
+  </si>
+  <si>
+    <t>[[MP: 1 ]]</t>
+  </si>
+  <si>
+    <t>[[Range: 1-2 ]]</t>
+  </si>
+  <si>
+    <t>[[Number of turns between two casts: 8 ]]</t>
+  </si>
+  <si>
+    <t>Summon a ''Canis Lupus'' [[25% of hunter max HP, 5 AP, 5 MP, 30% earth resistence, -10% fire resistence, -30% water resistence, 10% air resistence, -30% light resistence, 30% dark resistence]]</t>
+  </si>
+  <si>
+    <t>Usable only If not under ''Treason'' effect</t>
+  </si>
+  <si>
+    <t>Probably the only living thing that appreciate you.</t>
+  </si>
+  <si>
+    <t>Canis Lupus spells</t>
+  </si>
+  <si>
+    <t>Infected Bite</t>
+  </si>
+  <si>
+    <t>An infected bite, as if being bitten wasn't enough.</t>
+  </si>
+  <si>
+    <t>[[Range: 1 ]]</t>
+  </si>
+  <si>
+    <t>[[Max effect accumulation: 2 ]]</t>
+  </si>
+  <si>
+    <t>[[Damage:  5-10 earth ]]                                                      [[Damage:  20 dark ]] (2 turns)</t>
+  </si>
+  <si>
+    <t>The poison damage are triggered at the start of the target turn.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -328,6 +430,14 @@
       <color theme="1"/>
       <name val="Algerian"/>
       <family val="5"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -362,7 +472,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -416,11 +526,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -453,6 +587,19 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -939,7 +1086,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D33"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -1157,7 +1304,7 @@
   <dimension ref="B2:D29"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1735,7 +1882,7 @@
   <dimension ref="B2:D29"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1923,10 +2070,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D31"/>
+  <dimension ref="B2:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1958,167 +2105,160 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="C13" s="3"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3"/>
+      <c r="C14" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3" t="s">
-        <v>25</v>
+      <c r="C15" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="7" t="s">
-        <v>78</v>
-      </c>
+      <c r="C16" s="3"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="3"/>
+      <c r="C17" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
-      <c r="C18" s="3" t="s">
-        <v>79</v>
-      </c>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+      <c r="C19" s="13" t="s">
+        <v>83</v>
+      </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
-      <c r="C20" s="13" t="s">
-        <v>83</v>
+      <c r="C20" s="15" t="s">
+        <v>82</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="15" t="s">
-        <v>82</v>
+      <c r="C21" s="14" t="s">
+        <v>81</v>
       </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
-      <c r="C22" s="14" t="s">
-        <v>81</v>
+      <c r="C22" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
-      <c r="C23" s="3" t="s">
-        <v>84</v>
-      </c>
+      <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="C26" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
-      <c r="C27" s="5" t="s">
-        <v>10</v>
-      </c>
+      <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
+      <c r="C28" s="10" t="s">
+        <v>80</v>
+      </c>
       <c r="D28" s="1"/>
     </row>
     <row r="29" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B29" s="1"/>
       <c r="C29" s="10" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
-      <c r="C30" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="6"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2128,10 +2268,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D31"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2151,7 +2291,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>86</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2163,14 +2303,14 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>95</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B6" s="1"/>
       <c r="C6" s="9" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="D6" s="1"/>
     </row>
@@ -2182,160 +2322,146 @@
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>1</v>
+        <v>91</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="C10" s="3"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="7" t="s">
+        <v>88</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="C16" s="3"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C19" s="3"/>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="3" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
       <c r="C22" s="3" t="s">
-        <v>9</v>
+        <v>92</v>
       </c>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
+    <row r="25" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B27" s="1"/>
+      <c r="C27" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="1"/>
+    </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
+      <c r="C29" s="10" t="s">
+        <v>94</v>
       </c>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
+      <c r="C30" s="10" t="s">
+        <v>119</v>
+      </c>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2345,10 +2471,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D26"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2368,7 +2494,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>98</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2380,40 +2506,38 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>97</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>2</v>
+        <v>57</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -2425,71 +2549,63 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>101</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
+      <c r="C13" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
+      <c r="C22" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -2500,59 +2616,22 @@
     </row>
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
+      <c r="C24" s="10" t="s">
+        <v>104</v>
       </c>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
+      <c r="C25" s="10" t="s">
+        <v>105</v>
       </c>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="D26" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2562,214 +2641,277 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B1:H27"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
-    <col min="4" max="6" width="2.85546875" customWidth="1"/>
+    <col min="4" max="4" width="2.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="2.85546875" customWidth="1"/>
     <col min="7" max="7" width="78.5703125" customWidth="1"/>
     <col min="8" max="8" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="1"/>
+      <c r="G1" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="2:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>106</v>
       </c>
       <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F3" s="1"/>
+      <c r="G3" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="F4" s="1"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>112</v>
       </c>
       <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="F5" s="1"/>
+      <c r="G5" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="F7" s="1"/>
+      <c r="G7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>107</v>
       </c>
       <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="F8" s="1"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>1</v>
+        <v>108</v>
       </c>
       <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="F9" s="1"/>
+      <c r="G9" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="C10" s="3"/>
       <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="F10" s="1"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="F11" s="1"/>
+      <c r="G11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="F12" s="1"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="F13" s="1"/>
+      <c r="G13" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="F14" s="1"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>109</v>
+      </c>
       <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="F15" s="1"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="C16" s="3"/>
       <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="F16" s="1"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="F17" s="1"/>
+      <c r="G17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="2:8" ht="78" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
+      <c r="C19" s="17" t="s">
+        <v>110</v>
       </c>
       <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="F19" s="1"/>
+      <c r="G19" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="2:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="2:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="F23" s="1"/>
+      <c r="G23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
+      <c r="C25" s="10" t="s">
+        <v>111</v>
       </c>
       <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F25" s="1"/>
+      <c r="G25" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="D26" s="20"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="H26" s="20"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C27" s="19"/>
+      <c r="D27" s="21"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Hunter skills doc done.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/Hunter/Documentation/HunterSkills.xlsx
+++ b/GameDesign/Class/Hunter/Documentation/HunterSkills.xlsx
@@ -21,7 +21,7 @@
     <sheet name="7-PoisonArrow" sheetId="7" r:id="rId7"/>
     <sheet name="8-Survival" sheetId="8" r:id="rId8"/>
     <sheet name="9-CanisLupus" sheetId="9" r:id="rId9"/>
-    <sheet name="Feuil1 (10)" sheetId="10" r:id="rId10"/>
+    <sheet name="10-LastResort" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -33,65 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="120">
-  <si>
-    <t>[[AP: 0 ]]</t>
-  </si>
-  <si>
-    <t>[[MP: 0 ]]</t>
-  </si>
-  <si>
-    <t>[[Range: 0-0 ]]</t>
-  </si>
-  <si>
-    <t>[[Cast in straight line: - ]]</t>
-  </si>
-  <si>
-    <t>[[Modifiable range: - ]]</t>
-  </si>
-  <si>
-    <t>[[Number of casts per turn: - ]]</t>
-  </si>
-  <si>
-    <t>[[Number of cast per turn per target: - ]]</t>
-  </si>
-  <si>
-    <t>[[Max effect accumulation: - ]]</t>
-  </si>
-  <si>
-    <t>[[Line of sight: - ]]</t>
-  </si>
-  <si>
-    <t>[[Area of effect: - Stright line of 1 cell]]</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="110">
   <si>
     <t>Additional Info</t>
   </si>
   <si>
-    <t>[[Damage:  0-0 fire ]]</t>
-  </si>
-  <si>
-    <t>EX: [[Boost taken damage by 10%]] (2 turns)</t>
-  </si>
-  <si>
-    <t>SKILL DESCRIPTION</t>
-  </si>
-  <si>
-    <t>¨¨ ¨¨</t>
-  </si>
-  <si>
-    <t>SKILL NAME</t>
-  </si>
-  <si>
-    <t>Effect name: ''X''.</t>
-  </si>
-  <si>
-    <t>Unbuff ''X'' effect.</t>
-  </si>
-  <si>
-    <t>[[Number of turns between two casts: -  ]]</t>
-  </si>
-  <si>
     <t>Distortion Area</t>
   </si>
   <si>
@@ -393,6 +339,30 @@
   </si>
   <si>
     <t>The poison damage are triggered at the start of the target turn.</t>
+  </si>
+  <si>
+    <t>Last Resort</t>
+  </si>
+  <si>
+    <t>Effect name: ''Treason''.</t>
+  </si>
+  <si>
+    <t>Can only target ''Canis Lupus''.</t>
+  </si>
+  <si>
+    <t>Self: [[Heal:  The max HP of ''Canis Lupus'' ]]</t>
+  </si>
+  <si>
+    <t>Self: [[Treason effect ]] (00 turns)</t>
+  </si>
+  <si>
+    <t>Target: Unsummon ''Canis Lupus''.</t>
+  </si>
+  <si>
+    <t>[[Number of turns between two casts: 00 ]]</t>
+  </si>
+  <si>
+    <t>It's you or me, sorry buddy.</t>
   </si>
 </sst>
 </file>
@@ -937,7 +907,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -949,7 +919,7 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -961,14 +931,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -980,21 +950,21 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -1006,7 +976,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1018,7 +988,7 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -1030,7 +1000,7 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="3" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -1048,7 +1018,7 @@
     <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
       <c r="C22" s="5" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -1060,14 +1030,14 @@
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
       <c r="C24" s="10" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
       <c r="C25" s="10" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -1084,10 +1054,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1107,7 +1077,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>102</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1119,66 +1089,64 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>109</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>89</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="C10" s="3"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="C12" s="3"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>108</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
+      <c r="C14" s="7" t="s">
+        <v>60</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1190,108 +1158,77 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>105</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="3" t="s">
-        <v>5</v>
+        <v>106</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="3" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="1"/>
-    </row>
+    <row r="22" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
+      <c r="C24" s="5" t="s">
+        <v>0</v>
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="C26" s="10" t="s">
+        <v>103</v>
+      </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B27" s="1"/>
+      <c r="C27" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D27" s="1"/>
+    </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="D28" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1324,7 +1261,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1336,14 +1273,14 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B6" s="1"/>
       <c r="C6" s="9" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D6" s="1"/>
     </row>
@@ -1355,14 +1292,14 @@
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -1374,21 +1311,21 @@
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -1400,7 +1337,7 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="3" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -1412,14 +1349,14 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="3" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="3" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -1431,14 +1368,14 @@
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="3" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
       <c r="C21" s="3" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -1456,7 +1393,7 @@
     <row r="25" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
       <c r="C25" s="5" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -1468,14 +1405,14 @@
     <row r="27" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B27" s="1"/>
       <c r="C27" s="11" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="D27" s="1"/>
     </row>
     <row r="28" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B28" s="1"/>
       <c r="C28" s="11" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="D28" s="1"/>
     </row>
@@ -1515,7 +1452,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1527,14 +1464,14 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B6" s="1"/>
       <c r="C6" s="9" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="D6" s="1"/>
     </row>
@@ -1546,14 +1483,14 @@
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -1565,21 +1502,21 @@
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -1591,7 +1528,7 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="7" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -1603,7 +1540,7 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="3" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -1615,14 +1552,14 @@
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="3" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="3" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="D20" s="1"/>
     </row>
@@ -1634,21 +1571,21 @@
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
       <c r="C22" s="3" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
       <c r="C23" s="3" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
       <c r="C24" s="3" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="D24" s="1"/>
     </row>
@@ -1666,7 +1603,7 @@
     <row r="28" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B28" s="1"/>
       <c r="C28" s="5" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D28" s="1"/>
     </row>
@@ -1678,21 +1615,21 @@
     <row r="30" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B30" s="1"/>
       <c r="C30" s="11" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="D30" s="1"/>
     </row>
     <row r="31" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B31" s="1"/>
       <c r="C31" s="11" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="D31" s="1"/>
     </row>
     <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B32" s="1"/>
       <c r="C32" s="11" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="D32" s="1"/>
     </row>
@@ -1732,7 +1669,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1744,7 +1681,7 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1756,14 +1693,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1775,21 +1712,21 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -1801,7 +1738,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1813,7 +1750,7 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -1825,7 +1762,7 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="3" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -1843,7 +1780,7 @@
     <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
       <c r="C22" s="5" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -1855,14 +1792,14 @@
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
       <c r="C24" s="10" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
       <c r="C25" s="10" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -1902,7 +1839,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1914,14 +1851,14 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B6" s="1"/>
       <c r="C6" s="9" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="D6" s="1"/>
     </row>
@@ -1933,14 +1870,14 @@
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -1952,21 +1889,21 @@
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -1978,7 +1915,7 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="3" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -1990,14 +1927,14 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="3" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="3" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -2009,21 +1946,21 @@
     <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
       <c r="C20" s="3" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
       <c r="C21" s="13" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
       <c r="C22" s="14" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -2041,7 +1978,7 @@
     <row r="26" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B26" s="1"/>
       <c r="C26" s="5" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D26" s="1"/>
     </row>
@@ -2053,7 +1990,7 @@
     <row r="28" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B28" s="1"/>
       <c r="C28" s="12" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="D28" s="1"/>
     </row>
@@ -2093,7 +2030,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2105,7 +2042,7 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2117,14 +2054,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -2136,21 +2073,21 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -2162,14 +2099,14 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="7" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -2181,7 +2118,7 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="3" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -2193,28 +2130,28 @@
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="13" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="15" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
       <c r="C21" s="14" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
       <c r="C22" s="3" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -2232,7 +2169,7 @@
     <row r="26" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B26" s="1"/>
       <c r="C26" s="5" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D26" s="1"/>
     </row>
@@ -2244,14 +2181,14 @@
     <row r="28" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B28" s="1"/>
       <c r="C28" s="10" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="D28" s="1"/>
     </row>
     <row r="29" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B29" s="1"/>
       <c r="C29" s="10" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="D29" s="1"/>
     </row>
@@ -2291,7 +2228,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2303,14 +2240,14 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B6" s="1"/>
       <c r="C6" s="9" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="D6" s="1"/>
     </row>
@@ -2322,14 +2259,14 @@
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -2341,21 +2278,21 @@
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -2367,7 +2304,7 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="7" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -2379,14 +2316,14 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="3" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="3" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -2398,7 +2335,7 @@
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="3" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="D20" s="1"/>
     </row>
@@ -2410,14 +2347,14 @@
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
       <c r="C22" s="3" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
       <c r="C23" s="3" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="D23" s="1"/>
     </row>
@@ -2435,7 +2372,7 @@
     <row r="27" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B27" s="1"/>
       <c r="C27" s="5" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D27" s="1"/>
     </row>
@@ -2447,14 +2384,14 @@
     <row r="29" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B29" s="1"/>
       <c r="C29" s="10" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="D29" s="1"/>
     </row>
     <row r="30" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B30" s="1"/>
       <c r="C30" s="10" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="D30" s="1"/>
     </row>
@@ -2494,7 +2431,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2506,7 +2443,7 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2518,14 +2455,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -2537,7 +2474,7 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -2549,14 +2486,14 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="7" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -2568,7 +2505,7 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="3" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -2580,14 +2517,14 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="3" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="3" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -2605,7 +2542,7 @@
     <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
       <c r="C22" s="5" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -2617,14 +2554,14 @@
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
       <c r="C24" s="10" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
       <c r="C25" s="10" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -2644,7 +2581,7 @@
   <dimension ref="B1:H27"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2661,7 +2598,7 @@
     <row r="1" spans="2:8" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F1" s="1"/>
       <c r="G1" s="16" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="H1" s="1"/>
     </row>
@@ -2676,12 +2613,12 @@
     <row r="3" spans="2:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="D3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="8" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -2696,12 +2633,12 @@
     <row r="5" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="D5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="2" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -2716,19 +2653,19 @@
     <row r="7" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="D7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="3" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="D8" s="1"/>
       <c r="F8" s="1"/>
@@ -2738,12 +2675,12 @@
     <row r="9" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="D9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="3" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="H9" s="1"/>
     </row>
@@ -2758,19 +2695,19 @@
     <row r="11" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="D11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="3" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D12" s="1"/>
       <c r="F12" s="1"/>
@@ -2780,12 +2717,12 @@
     <row r="13" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="7" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="H13" s="1"/>
     </row>
@@ -2800,7 +2737,7 @@
     <row r="15" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="3" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="D15" s="1"/>
       <c r="F15" s="1"/>
@@ -2818,12 +2755,12 @@
     <row r="17" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="3" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="D17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="3" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="H17" s="1"/>
     </row>
@@ -2838,12 +2775,12 @@
     <row r="19" spans="2:8" ht="78" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="C19" s="17" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="D19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="18" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="H19" s="1"/>
     </row>
@@ -2867,12 +2804,12 @@
     <row r="23" spans="2:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
       <c r="C23" s="5" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="5" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H23" s="1"/>
     </row>
@@ -2887,12 +2824,12 @@
     <row r="25" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
       <c r="C25" s="10" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="D25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="10" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="H25" s="1"/>
     </row>
@@ -2902,7 +2839,7 @@
       <c r="D26" s="20"/>
       <c r="F26" s="1"/>
       <c r="G26" s="10" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="H26" s="20"/>
     </row>

</xml_diff>

<commit_message>
Added 5 news skills in the Guardian doc.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/Hunter/Documentation/HunterSkills.xlsx
+++ b/GameDesign/Class/Hunter/Documentation/HunterSkills.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="1" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="1-DistortionArea" sheetId="1" r:id="rId1"/>
@@ -320,9 +320,6 @@
     <t>Probably the only living thing that appreciate you.</t>
   </si>
   <si>
-    <t>Canis Lupus spells</t>
-  </si>
-  <si>
     <t>Infected Bite</t>
   </si>
   <si>
@@ -363,6 +360,9 @@
   </si>
   <si>
     <t>It's you or me, sorry buddy.</t>
+  </si>
+  <si>
+    <t>Canis Lupus skill</t>
   </si>
 </sst>
 </file>
@@ -887,7 +887,7 @@
   <dimension ref="B2:D26"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1056,7 +1056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -1077,7 +1077,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1089,7 +1089,7 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1115,7 +1115,7 @@
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -1139,7 +1139,7 @@
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -1170,21 +1170,21 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D20" s="1"/>
     </row>
@@ -1214,14 +1214,14 @@
     <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
       <c r="C26" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D26" s="1"/>
     </row>
     <row r="27" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B27" s="1"/>
       <c r="C27" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D27" s="1"/>
     </row>
@@ -2391,7 +2391,7 @@
     <row r="30" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B30" s="1"/>
       <c r="C30" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D30" s="1"/>
     </row>
@@ -2580,8 +2580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H27"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2598,7 +2598,7 @@
     <row r="1" spans="2:8" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F1" s="1"/>
       <c r="G1" s="16" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="H1" s="1"/>
     </row>
@@ -2618,7 +2618,7 @@
       <c r="D3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -2638,7 +2638,7 @@
       <c r="D5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -2680,7 +2680,7 @@
       <c r="D9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H9" s="1"/>
     </row>
@@ -2722,7 +2722,7 @@
       <c r="D13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H13" s="1"/>
     </row>
@@ -2780,7 +2780,7 @@
       <c r="D19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H19" s="1"/>
     </row>
@@ -2839,7 +2839,7 @@
       <c r="D26" s="20"/>
       <c r="F26" s="1"/>
       <c r="G26" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H26" s="20"/>
     </row>

</xml_diff>